<commit_message>
I think I've added them all..
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AF940-4E36-F940-805D-FAA6E50D4678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2A99F1-C677-C146-8E2C-3D3E4E3E4D36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20120" yWindow="2220" windowWidth="35840" windowHeight="21940" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20120" yWindow="2220" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definition" sheetId="11" r:id="rId1"/>
@@ -1384,8 +1384,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1393,6 +1391,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1610,11 +1610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9E3160-B42C-BE40-AC73-EFC562B0D135}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
@@ -10048,8 +10051,8 @@
       <c r="E50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="30"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="33"/>
       <c r="H50" s="4" t="s">
         <v>30</v>
       </c>
@@ -10126,8 +10129,8 @@
       <c r="E52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="29"/>
-      <c r="G52" s="30"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -10838,8 +10841,8 @@
       <c r="E74" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F74" s="29"/>
-      <c r="G74" s="30"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="33"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -10906,8 +10909,8 @@
       <c r="E76" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="29"/>
-      <c r="G76" s="30"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="33"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -11007,8 +11010,8 @@
       <c r="E79" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F79" s="29"/>
-      <c r="G79" s="30"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="33"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -27227,26 +27230,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD70A127-873D-F443-A45A-BEEE39B7A773}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="10.1640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" style="31" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="31" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="31" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="31" customWidth="1"/>
-    <col min="9" max="10" width="17.5" style="31" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="11" style="31" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" style="31" customWidth="1"/>
-    <col min="14" max="16" width="10.1640625" style="31" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" style="31" customWidth="1"/>
-    <col min="18" max="16384" width="12.6640625" style="31"/>
+    <col min="1" max="2" width="10.1640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="29" customWidth="1"/>
+    <col min="9" max="10" width="17.5" style="29" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="29" customWidth="1"/>
+    <col min="12" max="12" width="11" style="29" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="29" customWidth="1"/>
+    <col min="14" max="16" width="10.1640625" style="29" customWidth="1"/>
+    <col min="17" max="17" width="22.1640625" style="29" customWidth="1"/>
+    <col min="18" max="16384" width="12.6640625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.15">
@@ -27412,10 +27415,10 @@
       <c r="H5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="30" t="s">
         <v>339</v>
       </c>
       <c r="N5" s="11"/>
@@ -27443,10 +27446,10 @@
       <c r="H6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="30" t="s">
         <v>342</v>
       </c>
       <c r="N6" s="11"/>
@@ -27474,10 +27477,10 @@
       <c r="H7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="31" t="s">
         <v>345</v>
       </c>
       <c r="N7" s="11"/>

</xml_diff>

<commit_message>
IN-933 Add source condition for client and deputy phone numbers
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724248B-2611-2B48-88EF-7F0B4CF0E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E5B12-6ED8-0B47-A7EE-9B86347C6BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="344">
   <si>
     <t>table_name</t>
   </si>
@@ -1148,6 +1148,9 @@
   <si>
     <t>ACTIVE</t>
   </si>
+  <si>
+    <t>Client Phone = not null</t>
+  </si>
 </sst>
 </file>
 
@@ -1592,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D997D636-B97D-7B46-AB7B-633501338BD2}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1682,6 +1685,9 @@
       </c>
       <c r="F4" s="34" t="s">
         <v>339</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>343</v>
       </c>
       <c r="H4" s="34" t="s">
         <v>99</v>
@@ -1699,7 +1705,7 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
     </sheetView>
@@ -12342,7 +12348,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
set a default of none on feepayer_id
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2457D9-FE2C-5240-860F-242F4FF41AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B5ED95-9983-994F-A2A7-DF2620E35626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="344">
   <si>
     <t>table_name</t>
   </si>
@@ -1148,6 +1148,9 @@
   <si>
     <t>ACTIVE</t>
   </si>
+  <si>
+    <t>none</t>
+  </si>
 </sst>
 </file>
 
@@ -1698,7 +1701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
+      <selection pane="bottomLeft" activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3994,7 +3997,9 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
+      <c r="M69" s="4" t="s">
+        <v>343</v>
+      </c>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
       <c r="P69" s="4" t="s">

</xml_diff>